<commit_message>
fix data in excel file for correct import data to db
</commit_message>
<xml_diff>
--- a/study_program/importDataScript/data/IQAData.xlsx
+++ b/study_program/importDataScript/data/IQAData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\iqa_website_test\IQA-Website-for-KMITL-master\myvenv\Scripts\iqa_web\study_program\importDataScript\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\58090032\Desktop\iqa-kmitl-v2\study_program\importDataScript\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC7BA5A-419F-4204-98B8-25A9810C69DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program (ข้อมูลหลักสูตร)" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5711" uniqueCount="2464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5723" uniqueCount="2477">
   <si>
     <t>Program Name</t>
   </si>
@@ -7440,20 +7441,59 @@
     <t>VASUDO</t>
   </si>
   <si>
-    <t>TEMP</t>
-  </si>
-  <si>
-    <t>TEMP DEGREE</t>
-  </si>
-  <si>
-    <t>TEMP NAME</t>
+    <t>AGIFOODSCIDMT</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1OQUQx7U3xYDXGwqICPr_hTdpZkpuVQSj</t>
+  </si>
+  <si>
+    <t>หลักสูตรปรัชญาดุษฎีบัณฑิต สาขาวิชาวิทยาศาสตร์การอาหาร</t>
+  </si>
+  <si>
+    <t>ปรัชญาดุษฎีบัณฑิต (วิทยาศาสตร์การอาหาร)</t>
+  </si>
+  <si>
+    <t>AGIFOODSAFMMT</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=193LyAui9ZsAK7QGnr1deJVQIFYCK9hsq</t>
+  </si>
+  <si>
+    <t>หลักสูตรวิทยาศาสตรมหาบัณฑิต สาขาวิชาการจัดการความปลอดภัยอาหาร</t>
+  </si>
+  <si>
+    <t>วิทยาศาสตรมหาบัณฑิต (การจัดการความปลอดภัยอาหาร)</t>
+  </si>
+  <si>
+    <t>AGIFOODSERMMT</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1lPbnMUroUXOtVx6AIUgcVJ4AmQd1pffs</t>
+  </si>
+  <si>
+    <t>หลักสูตรวิทยาศาสตรมหาบัณฑิต สาขาวิชาเทคโนโลยีการบริการอาหารและการจัดการ</t>
+  </si>
+  <si>
+    <t>วิทยาศาสตรมหาบัณฑิต (เทคโนโลยีการบริการอาหารและการจัดการ)</t>
+  </si>
+  <si>
+    <t>AGIFOODSCIMMT</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16YZ7lCsqnGbLSixF4UiZtHNh5L7ZHBbt</t>
+  </si>
+  <si>
+    <t>หลักสูตรวิทยาศาสตรมหาบัณฑิต สาขาวิชาวิทยาศาสตร์อาหาร</t>
+  </si>
+  <si>
+    <t>วิทยาศาสตรมหาบัณฑิต (วิทยาศาสตร์อาหาร)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="47">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -7720,6 +7760,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -7882,7 +7929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -8302,7 +8349,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8582,14 +8633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z216"/>
+  <dimension ref="A1:Z215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D178" workbookViewId="0">
-      <selection activeCell="H189" sqref="H189"/>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12925,54 +12976,96 @@
       <c r="A189" s="191" t="s">
         <v>2461</v>
       </c>
-      <c r="B189" s="34" t="s">
-        <v>1527</v>
+      <c r="B189" s="192" t="s">
+        <v>2462</v>
       </c>
       <c r="C189" s="191" t="s">
         <v>2463</v>
       </c>
-      <c r="D189" s="191" t="s">
-        <v>2462</v>
-      </c>
-      <c r="E189" s="178">
-        <v>1</v>
-      </c>
-      <c r="F189" s="178">
-        <v>1</v>
-      </c>
-      <c r="G189" s="178">
+      <c r="D189" s="193" t="s">
+        <v>2464</v>
+      </c>
+      <c r="E189" s="16">
+        <v>1</v>
+      </c>
+      <c r="F189" s="16">
+        <v>1</v>
+      </c>
+      <c r="G189" s="16">
         <v>1</v>
       </c>
       <c r="H189" s="178"/>
     </row>
     <row r="190" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A190" s="178"/>
-      <c r="B190" s="178"/>
-      <c r="C190" s="178"/>
-      <c r="D190" s="178"/>
-      <c r="E190" s="178"/>
-      <c r="F190" s="178"/>
-      <c r="G190" s="178"/>
+      <c r="A190" s="191" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B190" s="192" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C190" s="191" t="s">
+        <v>2467</v>
+      </c>
+      <c r="D190" s="193" t="s">
+        <v>2468</v>
+      </c>
+      <c r="E190" s="16">
+        <v>1</v>
+      </c>
+      <c r="F190" s="16">
+        <v>1</v>
+      </c>
+      <c r="G190" s="16">
+        <v>1</v>
+      </c>
       <c r="H190" s="178"/>
     </row>
     <row r="191" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A191" s="178"/>
-      <c r="B191" s="178"/>
-      <c r="C191" s="178"/>
-      <c r="D191" s="178"/>
-      <c r="E191" s="178"/>
-      <c r="F191" s="178"/>
-      <c r="G191" s="178"/>
+      <c r="A191" s="191" t="s">
+        <v>2469</v>
+      </c>
+      <c r="B191" s="192" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C191" s="191" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D191" s="193" t="s">
+        <v>2472</v>
+      </c>
+      <c r="E191" s="16">
+        <v>1</v>
+      </c>
+      <c r="F191" s="16">
+        <v>1</v>
+      </c>
+      <c r="G191" s="16">
+        <v>1</v>
+      </c>
       <c r="H191" s="178"/>
     </row>
     <row r="192" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A192" s="178"/>
-      <c r="B192" s="178"/>
-      <c r="C192" s="178"/>
-      <c r="D192" s="178"/>
-      <c r="E192" s="178"/>
-      <c r="F192" s="178"/>
-      <c r="G192" s="178"/>
+      <c r="A192" s="191" t="s">
+        <v>2473</v>
+      </c>
+      <c r="B192" s="192" t="s">
+        <v>2474</v>
+      </c>
+      <c r="C192" s="191" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D192" s="193" t="s">
+        <v>2476</v>
+      </c>
+      <c r="E192" s="16">
+        <v>1</v>
+      </c>
+      <c r="F192" s="16">
+        <v>1</v>
+      </c>
+      <c r="G192" s="16">
+        <v>1</v>
+      </c>
       <c r="H192" s="178"/>
     </row>
     <row r="193" spans="1:8" ht="15.75" customHeight="1">
@@ -13015,25 +13108,25 @@
       <c r="G196" s="178"/>
       <c r="H196" s="178"/>
     </row>
-    <row r="197" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A197" s="178"/>
-      <c r="B197" s="178"/>
-      <c r="C197" s="178"/>
-      <c r="D197" s="178"/>
-      <c r="E197" s="178"/>
-      <c r="F197" s="178"/>
-      <c r="G197" s="178"/>
-      <c r="H197" s="178"/>
-    </row>
-    <row r="198" spans="1:8" s="177" customFormat="1" ht="21">
-      <c r="A198" s="179"/>
-      <c r="B198" s="179"/>
-      <c r="C198" s="180"/>
-      <c r="D198" s="181"/>
-      <c r="E198" s="179"/>
-      <c r="F198" s="179"/>
-      <c r="G198" s="179"/>
-      <c r="H198" s="182"/>
+    <row r="197" spans="1:8" s="177" customFormat="1" ht="21">
+      <c r="A197" s="179"/>
+      <c r="B197" s="179"/>
+      <c r="C197" s="180"/>
+      <c r="D197" s="181"/>
+      <c r="E197" s="179"/>
+      <c r="F197" s="179"/>
+      <c r="G197" s="179"/>
+      <c r="H197" s="182"/>
+    </row>
+    <row r="198" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A198" s="178"/>
+      <c r="B198" s="178"/>
+      <c r="C198" s="178"/>
+      <c r="D198" s="178"/>
+      <c r="E198" s="178"/>
+      <c r="F198" s="178"/>
+      <c r="G198" s="178"/>
+      <c r="H198" s="178"/>
     </row>
     <row r="199" spans="1:8" ht="15.75" customHeight="1">
       <c r="A199" s="178"/>
@@ -13185,238 +13278,231 @@
       <c r="G213" s="178"/>
       <c r="H213" s="178"/>
     </row>
-    <row r="214" spans="1:8" ht="15.75" customHeight="1">
+    <row r="214" spans="1:8" ht="21">
       <c r="A214" s="178"/>
       <c r="B214" s="178"/>
-      <c r="C214" s="178"/>
+      <c r="C214" s="183"/>
       <c r="D214" s="178"/>
       <c r="E214" s="178"/>
       <c r="F214" s="178"/>
       <c r="G214" s="178"/>
       <c r="H214" s="178"/>
     </row>
-    <row r="215" spans="1:8" ht="21">
+    <row r="215" spans="1:8" ht="15.75" customHeight="1">
       <c r="A215" s="178"/>
       <c r="B215" s="178"/>
-      <c r="C215" s="183"/>
+      <c r="C215" s="178"/>
       <c r="D215" s="178"/>
       <c r="E215" s="178"/>
       <c r="F215" s="178"/>
       <c r="G215" s="178"/>
       <c r="H215" s="178"/>
     </row>
-    <row r="216" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A216" s="178"/>
-      <c r="B216" s="178"/>
-      <c r="C216" s="178"/>
-      <c r="D216" s="178"/>
-      <c r="E216" s="178"/>
-      <c r="F216" s="178"/>
-      <c r="G216" s="178"/>
-      <c r="H216" s="178"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-    <hyperlink ref="B32" r:id="rId30"/>
-    <hyperlink ref="B33" r:id="rId31"/>
-    <hyperlink ref="B34" r:id="rId32"/>
-    <hyperlink ref="B35" r:id="rId33"/>
-    <hyperlink ref="B36" r:id="rId34"/>
-    <hyperlink ref="B37" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
-    <hyperlink ref="B41" r:id="rId39"/>
-    <hyperlink ref="B42" r:id="rId40"/>
-    <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B44" r:id="rId42"/>
-    <hyperlink ref="B45" r:id="rId43"/>
-    <hyperlink ref="B46" r:id="rId44"/>
-    <hyperlink ref="B47" r:id="rId45"/>
-    <hyperlink ref="B48" r:id="rId46"/>
-    <hyperlink ref="B49" r:id="rId47"/>
-    <hyperlink ref="B50" r:id="rId48"/>
-    <hyperlink ref="B51" r:id="rId49"/>
-    <hyperlink ref="B52" r:id="rId50"/>
-    <hyperlink ref="B53" r:id="rId51"/>
-    <hyperlink ref="B54" r:id="rId52"/>
-    <hyperlink ref="B55" r:id="rId53"/>
-    <hyperlink ref="B56" r:id="rId54"/>
-    <hyperlink ref="B57" r:id="rId55"/>
-    <hyperlink ref="B58" r:id="rId56"/>
-    <hyperlink ref="B59" r:id="rId57"/>
-    <hyperlink ref="B60" r:id="rId58"/>
-    <hyperlink ref="B61" r:id="rId59"/>
-    <hyperlink ref="B62" r:id="rId60"/>
-    <hyperlink ref="B63" r:id="rId61"/>
-    <hyperlink ref="B64" r:id="rId62"/>
-    <hyperlink ref="B65" r:id="rId63"/>
-    <hyperlink ref="B66" r:id="rId64"/>
-    <hyperlink ref="B67" r:id="rId65"/>
-    <hyperlink ref="B68" r:id="rId66"/>
-    <hyperlink ref="B69" r:id="rId67"/>
-    <hyperlink ref="B70" r:id="rId68"/>
-    <hyperlink ref="B71" r:id="rId69"/>
-    <hyperlink ref="B72" r:id="rId70"/>
-    <hyperlink ref="B73" r:id="rId71"/>
-    <hyperlink ref="B74" r:id="rId72"/>
-    <hyperlink ref="B75" r:id="rId73"/>
-    <hyperlink ref="B76" r:id="rId74"/>
-    <hyperlink ref="B77" r:id="rId75"/>
-    <hyperlink ref="B78" r:id="rId76"/>
-    <hyperlink ref="B79" r:id="rId77"/>
-    <hyperlink ref="B80" r:id="rId78"/>
-    <hyperlink ref="B81" r:id="rId79"/>
-    <hyperlink ref="B82" r:id="rId80"/>
-    <hyperlink ref="B83" r:id="rId81"/>
-    <hyperlink ref="B84" r:id="rId82"/>
-    <hyperlink ref="B85" r:id="rId83"/>
-    <hyperlink ref="B86" r:id="rId84"/>
-    <hyperlink ref="B87" r:id="rId85"/>
-    <hyperlink ref="B88" r:id="rId86"/>
-    <hyperlink ref="B89" r:id="rId87"/>
-    <hyperlink ref="B90" r:id="rId88"/>
-    <hyperlink ref="B91" r:id="rId89"/>
-    <hyperlink ref="B92" r:id="rId90"/>
-    <hyperlink ref="B93" r:id="rId91"/>
-    <hyperlink ref="B94" r:id="rId92"/>
-    <hyperlink ref="B95" r:id="rId93"/>
-    <hyperlink ref="B96" r:id="rId94"/>
-    <hyperlink ref="B97" r:id="rId95"/>
-    <hyperlink ref="B98" r:id="rId96"/>
-    <hyperlink ref="B99" r:id="rId97"/>
-    <hyperlink ref="B100" r:id="rId98"/>
-    <hyperlink ref="B101" r:id="rId99"/>
-    <hyperlink ref="B102" r:id="rId100"/>
-    <hyperlink ref="B103" r:id="rId101"/>
-    <hyperlink ref="B104" r:id="rId102"/>
-    <hyperlink ref="B105" r:id="rId103"/>
-    <hyperlink ref="B106" r:id="rId104"/>
-    <hyperlink ref="B107" r:id="rId105"/>
-    <hyperlink ref="B108" r:id="rId106"/>
-    <hyperlink ref="B109" r:id="rId107"/>
-    <hyperlink ref="B110" r:id="rId108"/>
-    <hyperlink ref="B111" r:id="rId109"/>
-    <hyperlink ref="B112" r:id="rId110"/>
-    <hyperlink ref="B113" r:id="rId111"/>
-    <hyperlink ref="B114" r:id="rId112"/>
-    <hyperlink ref="B115" r:id="rId113"/>
-    <hyperlink ref="B116" r:id="rId114"/>
-    <hyperlink ref="B117" r:id="rId115"/>
-    <hyperlink ref="B118" r:id="rId116"/>
-    <hyperlink ref="B119" r:id="rId117"/>
-    <hyperlink ref="B120" r:id="rId118"/>
-    <hyperlink ref="B121" r:id="rId119"/>
-    <hyperlink ref="B122" r:id="rId120"/>
-    <hyperlink ref="B123" r:id="rId121"/>
-    <hyperlink ref="B124" r:id="rId122"/>
-    <hyperlink ref="B125" r:id="rId123"/>
-    <hyperlink ref="B126" r:id="rId124"/>
-    <hyperlink ref="B127" r:id="rId125"/>
-    <hyperlink ref="B128" r:id="rId126"/>
-    <hyperlink ref="B129" r:id="rId127"/>
-    <hyperlink ref="B130" r:id="rId128"/>
-    <hyperlink ref="B131" r:id="rId129"/>
-    <hyperlink ref="B132" r:id="rId130"/>
-    <hyperlink ref="B133" r:id="rId131"/>
-    <hyperlink ref="B134" r:id="rId132"/>
-    <hyperlink ref="B135" r:id="rId133"/>
-    <hyperlink ref="B136" r:id="rId134"/>
-    <hyperlink ref="B137" r:id="rId135"/>
-    <hyperlink ref="B138" r:id="rId136"/>
-    <hyperlink ref="B139" r:id="rId137"/>
-    <hyperlink ref="B140" r:id="rId138"/>
-    <hyperlink ref="B141" r:id="rId139"/>
-    <hyperlink ref="B142" r:id="rId140"/>
-    <hyperlink ref="B143" r:id="rId141"/>
-    <hyperlink ref="B144" r:id="rId142"/>
-    <hyperlink ref="B145" r:id="rId143"/>
-    <hyperlink ref="B146" r:id="rId144"/>
-    <hyperlink ref="B147" r:id="rId145"/>
-    <hyperlink ref="B148" r:id="rId146"/>
-    <hyperlink ref="B149" r:id="rId147"/>
-    <hyperlink ref="B150" r:id="rId148"/>
-    <hyperlink ref="B151" r:id="rId149"/>
-    <hyperlink ref="B152" r:id="rId150"/>
-    <hyperlink ref="B153" r:id="rId151"/>
-    <hyperlink ref="B154" r:id="rId152"/>
-    <hyperlink ref="B155" r:id="rId153"/>
-    <hyperlink ref="B156" r:id="rId154"/>
-    <hyperlink ref="B157" r:id="rId155"/>
-    <hyperlink ref="B158" r:id="rId156"/>
-    <hyperlink ref="B159" r:id="rId157"/>
-    <hyperlink ref="B160" r:id="rId158"/>
-    <hyperlink ref="B161" r:id="rId159"/>
-    <hyperlink ref="B162" r:id="rId160"/>
-    <hyperlink ref="B163" r:id="rId161"/>
-    <hyperlink ref="B164" r:id="rId162"/>
-    <hyperlink ref="B165" r:id="rId163"/>
-    <hyperlink ref="B166" r:id="rId164"/>
-    <hyperlink ref="B167" r:id="rId165"/>
-    <hyperlink ref="B168" r:id="rId166"/>
-    <hyperlink ref="B169" r:id="rId167"/>
-    <hyperlink ref="B170" r:id="rId168"/>
-    <hyperlink ref="B171" r:id="rId169"/>
-    <hyperlink ref="B172" r:id="rId170"/>
-    <hyperlink ref="B173" r:id="rId171"/>
-    <hyperlink ref="B174" r:id="rId172"/>
-    <hyperlink ref="B175" r:id="rId173"/>
-    <hyperlink ref="B176" r:id="rId174"/>
-    <hyperlink ref="B177" r:id="rId175"/>
-    <hyperlink ref="B178" r:id="rId176"/>
-    <hyperlink ref="B179" r:id="rId177"/>
-    <hyperlink ref="B180" r:id="rId178"/>
-    <hyperlink ref="B181" r:id="rId179"/>
-    <hyperlink ref="B182" r:id="rId180"/>
-    <hyperlink ref="B183" r:id="rId181"/>
-    <hyperlink ref="B184" r:id="rId182"/>
-    <hyperlink ref="B185" r:id="rId183"/>
-    <hyperlink ref="B186" r:id="rId184"/>
-    <hyperlink ref="B187" r:id="rId185"/>
-    <hyperlink ref="B188" r:id="rId186"/>
-    <hyperlink ref="B189" r:id="rId187"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B74" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B75" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B76" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B77" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B78" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B79" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B80" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B81" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B85" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B87" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B88" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B92" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B94" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B96" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B97" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B98" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B99" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B101" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B102" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B103" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B104" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B106" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B107" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B108" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B109" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B110" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B112" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B113" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B114" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B115" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B116" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B117" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B118" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B119" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B120" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B121" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B122" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B123" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B124" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B125" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B126" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B127" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B128" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B129" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B130" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B131" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B132" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B133" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B134" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B135" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B136" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B137" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B138" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B139" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B140" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B141" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B142" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B143" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B144" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B145" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B146" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B147" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B148" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B149" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B150" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B151" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B152" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B153" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B154" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B155" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B156" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B157" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B158" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B159" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B160" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B161" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B162" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B163" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B164" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B165" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B166" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B167" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B168" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B169" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B170" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B171" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B172" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B173" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B174" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B175" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B176" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B177" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B178" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B179" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B180" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B181" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B182" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B183" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B184" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B185" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B186" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B187" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B188" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B189" r:id="rId187" xr:uid="{A5A53BD1-146E-41FA-99D9-50BDCB27452F}"/>
+    <hyperlink ref="B190" r:id="rId188" xr:uid="{5308DA1B-C59D-4FC0-AE4A-D4A4B6D934E3}"/>
+    <hyperlink ref="B191" r:id="rId189" xr:uid="{DCA576F8-4B2B-45EB-8755-6500B6A74F5A}"/>
+    <hyperlink ref="B192" r:id="rId190" xr:uid="{FDB0C5C0-1F9C-48CB-9959-3571141E2FD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z776"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A759" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -23616,13 +23702,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D769"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A754" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -32099,7 +32185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32380,13 +32466,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B322"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -34979,13 +35065,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -35334,14 +35422,14 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>